<commit_message>
fix VideoView cannot play in 2.3.6
auto mode S39H cannot play videoview
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="145">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -579,6 +579,33 @@
   </si>
   <si>
     <t>文件头损坏，需要做workaround</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.6手机 变形金刚 截图很容易失败</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[铁臂阿童木][Astro.Boy_48k.mp3 声音不对
+国际潜水小姐大赛.冠军专访.m2t
+D:\Archive\media\audio\邓紫棋 - 泡沫.flac
+D:\Archive\media\audio\陈慧娴-飘雪.ape</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -644,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -697,6 +724,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H25"/>
+  <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1521,9 +1551,46 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="3">
+      <c r="B25" s="7">
         <v>24</v>
       </c>
+      <c r="C25" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="15">
+        <v>20150123</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="B26" s="7">
+        <v>25</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="15">
+        <v>20150116</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
1 fix bug PPBOX-3178 tvplayer3.0 播放一mpg片源，有严重的噪音 2 win32 testDlg add cleanup()
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="157">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -313,19 +313,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>播放器选择策略重写</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>tscc解码器支持</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>view框架Mediaplayer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>待完善</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -523,14 +515,6 @@
   </si>
   <si>
     <t>armv7s xcodebuild NOT generated</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PhaseI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pre-release</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -606,6 +590,70 @@
 国际潜水小姐大赛.冠军专访.m2t
 D:\Archive\media\audio\邓紫棋 - 泡沫.flac
 D:\Archive\media\audio\陈慧娴-飘雪.ape</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://172.16.204.104/200438.mp4 播放很卡</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持代码混淆proguard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>release 1st stable version</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>re-write policy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>need enhance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3178</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>某些片子声音播放有很大噪声</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>audioFrame linezize &gt;= nbSample(2048 502)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -671,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -684,9 +732,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1029,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H26"/>
+  <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1086,7 @@
     <col min="2" max="2" width="9" style="3"/>
     <col min="3" max="3" width="13.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.75" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.75" style="12" customWidth="1"/>
     <col min="6" max="6" width="48.125" style="3" customWidth="1"/>
     <col min="7" max="7" width="8.875" style="3" customWidth="1"/>
     <col min="8" max="8" width="74.625" style="3" customWidth="1"/>
@@ -1058,8 +1103,8 @@
       <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>101</v>
+      <c r="E1" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
@@ -1102,7 +1147,7 @@
         <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>34</v>
@@ -1205,7 +1250,7 @@
         <v>59</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>60</v>
@@ -1262,7 +1307,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>34</v>
@@ -1270,47 +1315,47 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>11</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.3">
-      <c r="B13" s="7">
-        <v>12</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -1318,19 +1363,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -1338,19 +1383,19 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -1358,150 +1403,151 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.3">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="G17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H18" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="15">
+        <v>18</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="9">
+        <v>19</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="13">
+        <v>20150107</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="7">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="16">
-        <v>18</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="10">
-        <v>19</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="14">
-        <v>20150107</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="7">
-        <v>20</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="E21" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="15" t="s">
+      <c r="G21" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="9">
+        <v>21</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="D22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="13">
+        <v>20150115</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="10">
-        <v>21</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="G22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="E22" s="14">
-        <v>20150115</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -1509,93 +1555,203 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="12">
+        <v>20150122</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" s="13">
-        <v>20150122</v>
-      </c>
-      <c r="F23" s="3" t="s">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="6">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="14">
+        <v>20150121</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="7">
-        <v>23</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="15">
-        <v>20150121</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="H24" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="6">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="7">
-        <v>24</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="E25" s="14">
+        <v>20150123</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.3">
+      <c r="B26" s="6">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E26" s="14">
+        <v>20150116</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="15">
-        <v>20150123</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="G26" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="6">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="E27" s="14">
+        <v>20150127</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.3">
-      <c r="B26" s="7">
-        <v>25</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="7" t="s">
+      <c r="G27" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="15">
-        <v>20150116</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="H26" s="7"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="6">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="14">
+        <v>20150128</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="3">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F27" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <ignoredErrors>
     <ignoredError sqref="E12 E21" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -1607,7 +1763,7 @@
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1773,22 +1929,22 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
+      <c r="B7" s="6">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="2"/>
@@ -1845,22 +2001,22 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
+      <c r="B10" s="6">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="H10" s="2"/>
@@ -1923,20 +2079,20 @@
       <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>124</v>
+      <c r="F13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1959,7 +2115,7 @@
         <v>61</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2005,13 +2161,13 @@
         <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2025,7 +2181,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>64</v>
@@ -2045,19 +2201,19 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2070,19 +2226,19 @@
       <c r="B19" s="3">
         <v>18</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" s="10"/>
+      <c r="E19" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="9"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2095,13 +2251,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>34</v>
@@ -2118,10 +2274,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>34</v>
@@ -2136,6 +2292,18 @@
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>21</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>

</xml_diff>

<commit_message>
1 meetplayer implement dlna push_to_dmr 2 win32 testDlg support vlc play
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="170">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -654,6 +654,58 @@
   </si>
   <si>
     <t>audioFrame linezize &gt;= nbSample(2048 502)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>由于编译问题vc1解码模块disabled，导致vc1影片无法播放</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自有播放器播放 陈慧娴-飘雪.ape文件进度条走的很快，声音不对</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自有播放器播放 茜拉-想你的夜.WAV pos显示不对</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>扫描本地文件写入db</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1076,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1684,16 +1736,61 @@
       <c r="B29" s="3">
         <v>28</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="12">
+        <v>20150129</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="3">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
+      <c r="C30" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="14">
+        <v>20150129</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="3">
+      <c r="B31" s="6">
         <v>30</v>
       </c>
+      <c r="C31" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="14">
+        <v>20150129</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="3">
@@ -1762,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2315,6 +2412,18 @@
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>

</xml_diff>

<commit_message>
step2 1 fix play ape flac too fast problem 2 use "seek" in select audio track
known issue:
1 声音文件 seek会 回跳
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="179">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -681,10 +681,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>tracking</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>自有播放器播放 陈慧娴-飘雪.ape文件进度条走的很快，声音不对</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -730,6 +726,22 @@
   </si>
   <si>
     <t>fake audio clock</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>foundation_rext included</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>audio packet  包含多帧AVFrame数据,不能只读取第一个就退出</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1152,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1777,25 +1789,27 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="6">
+      <c r="B30" s="9">
         <v>29</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <v>20150129</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="F30" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="G30" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
@@ -1811,7 +1825,7 @@
         <v>20150129</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1883,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2308,7 +2322,10 @@
         <v>64</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>34</v>
+        <v>175</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -2438,16 +2455,16 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -2461,16 +2478,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2484,19 +2501,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="E25" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
step3 1 fix ape duration no correct problem 2 fix stop delay 500 msec problem
known issue:
1 xx.ape mp3(audio file) to switch to play video will stuck at loop.stop()
2 swr function need re-write(in out param)
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="186">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -754,6 +754,22 @@
   </si>
   <si>
     <t>seek ape文件 进度条 会"回跳"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取 cpu 是否是neon以支持自有播放器</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1176,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1925,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2547,6 +2563,18 @@
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <v>25</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 fix ffplay stayAwake 2 add wifilock in ClipListActivity.java
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="196">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -794,6 +794,22 @@
   </si>
   <si>
     <t>同29</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">没有在各个调用 设置stayAwake </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>播放中自动黑屏休眠了(系统播放器还没有解决)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1222,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1939,6 +1955,24 @@
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="3">
         <v>33</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" s="12">
+        <v>20150225</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 add meetvideoview test activity 2 fix multi-seek event just do once problem
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="201">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -805,11 +805,31 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">没有在各个调用 设置stayAwake </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>播放中自动黑屏休眠了(系统播放器还没有解决)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3170</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OTT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rmvb片源快进后声音异常</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有在start stop等 设置stayAwake, 增加了nativeplayer基类</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始播放后，seek到片子中段，会有杂音</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1238,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1966,18 +1986,36 @@
         <v>20150225</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="6">
+        <v>34</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="D35" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="14">
+        <v>20150225</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="G35" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="3">
-        <v>34</v>
+      <c r="H35" s="6" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 update Doc 2 modify Android.mk 3 modify subtitle 4 update tinyxml2 code from github leethomason/tinyxml2
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="239">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -908,6 +908,82 @@
   </si>
   <si>
     <t>见log ios8_hls_crash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PPBOX-3717 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OTT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DLNA推送在线视频，视频A播放完后播放视频B时，提示视频解析出错，实际可正常播放</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3706</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地播放.ogg音乐，不论播放控制选择什么，播放模式都是单个循环</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统播放器 没有 onComplete 回调？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3693</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外挂字幕的片源，播放时不会自动挂载字幕，手动加载也加载不上</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>老版sdk支持的srt字幕，现在不支持了</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wmv片源新sdk版本播放声音卡顿，旧sdk正常</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3417</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3695</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>播放多音轨片源 选择音轨2时，我的设备挂掉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>多音轨 各个音轨的channel_layout属性不同，需要重启audioplayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOS6系统 自有播放器 播放hls crash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ld error</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1334,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H41"/>
+  <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2145,23 +2221,182 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="3">
+      <c r="B38" s="6">
         <v>37</v>
       </c>
+      <c r="C38" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E38" s="14">
+        <v>20150320</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="3">
+      <c r="B39" s="6">
         <v>38</v>
       </c>
+      <c r="C39" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="14">
+        <v>20150320</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="3">
+      <c r="B40" s="6">
         <v>39</v>
       </c>
+      <c r="C40" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" s="14">
+        <v>20150320</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="3">
+      <c r="B41" s="6">
         <v>40</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E41" s="14">
+        <v>20150320</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="3">
+        <v>41</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" s="12">
+        <v>20150319</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="6">
+        <v>42</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E43" s="14">
+        <v>20150318</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="3">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
engine2 fix play some "ac3 5.1 channel clip" crash
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="267">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -857,14 +857,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>tracking</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>见log ios8_hls_crash</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">PPBOX-3717 </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -926,10 +918,6 @@
   </si>
   <si>
     <t>IOS6系统 自有播放器 播放hls crash</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ld error</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -996,6 +984,119 @@
   </si>
   <si>
     <t>合并 施版 loop代码，已修复</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 连续切换视频播放，一定几率loop卡死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用stop()加锁 loop线程退出时，有BufferingEnd SeekingComplete等
+回调时间触发，错误的加锁导致死锁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>播放某些ac3 5.1声道影片时 crash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>某些影片开头的解码AVFrame chanel_layout 属性会变化，导致swresample crash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wont fix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>见log ios8_hls_crash, xcode6 编译lib库对老版本ios支持不好</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>invalid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同36</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持内嵌字幕</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>内嵌字幕支持切换</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换后，需要等待一段时间，字幕才加载(原因 切字幕没有seek，导致字幕数据被丢弃)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>foundation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vp9 汇编优化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hongshen.zhao</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hongshen.zhao push to gitlab branch dev_vp9neon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>swscale 汇编优化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>doing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>support arm64</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>add x264 fdk-aac openssl librtmp speedx</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1061,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1119,6 +1220,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1424,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1598,7 +1702,7 @@
         <v>56</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>57</v>
@@ -1658,7 +1762,7 @@
         <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -1723,7 +1827,7 @@
         <v>114</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -1781,10 +1885,10 @@
         <v>90</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -1802,7 +1906,7 @@
         <v>92</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>93</v>
@@ -1869,7 +1973,7 @@
         <v>106</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>129</v>
@@ -2003,10 +2107,10 @@
         <v>137</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -2138,10 +2242,10 @@
         <v>180</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
@@ -2187,7 +2291,7 @@
         <v>125</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
@@ -2230,10 +2334,10 @@
         <v>206</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>208</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
@@ -2241,22 +2345,22 @@
         <v>37</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E38" s="14">
         <v>20150320</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
@@ -2264,22 +2368,22 @@
         <v>38</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E39" s="13">
         <v>20150320</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
@@ -2287,22 +2391,22 @@
         <v>39</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E40" s="13">
         <v>20150320</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
@@ -2310,22 +2414,22 @@
         <v>40</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E41" s="13">
         <v>20150320</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
@@ -2333,22 +2437,22 @@
         <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E42" s="12">
         <v>20150319</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
@@ -2356,32 +2460,68 @@
         <v>42</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E43" s="14">
         <v>20150318</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>125</v>
+        <v>247</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="3">
         <v>43</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" s="12">
+        <v>20150802</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
         <v>44</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E45" s="12">
+        <v>20150812</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
@@ -2434,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M30"/>
+  <dimension ref="B1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2616,10 +2756,10 @@
         <v>30</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2662,10 +2802,10 @@
         <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>36</v>
@@ -2691,10 +2831,10 @@
         <v>38</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2717,7 +2857,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2940,7 +3080,7 @@
         <v>76</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -2960,7 +3100,7 @@
         <v>77</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>33</v>
+        <v>251</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3052,7 +3192,7 @@
         <v>166</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>167</v>
@@ -3072,7 +3212,7 @@
         <v>176</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
@@ -3089,7 +3229,7 @@
         <v>200</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>203</v>
@@ -3119,10 +3259,121 @@
       <c r="B29" s="3">
         <v>28</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <v>29</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="3">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="3">
+        <v>32</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="3">
+        <v>33</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="3">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 meetsdk support MediaPlayer.reset() and play different url 2 foundation update build batch
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="271">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1097,6 +1097,22 @@
   </si>
   <si>
     <t>add x264 fdk-aac openssl librtmp speedx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>engine2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>support only video/audio play when codec unsupported</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2586,7 +2602,7 @@
     <col min="2" max="2" width="9" style="3"/>
     <col min="3" max="3" width="15.375" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="34.875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41.75" style="3" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" customWidth="1"/>
     <col min="7" max="7" width="64.25" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
@@ -3369,6 +3385,18 @@
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="3">
         <v>34</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 foundation add eac3(dd+) in "lite" build 2 engine2 fix some dts clip codecId is NONE
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="281">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -47,10 +47,6 @@
   </si>
   <si>
     <t>getState</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1084,10 +1080,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>doing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>meetsdk</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1113,6 +1105,54 @@
   </si>
   <si>
     <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>engine2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>media info add "codec profile" to support dts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wont do</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>look MoliPlayer implement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OMXPlayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>look ndk sample</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>system player support snapshot</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1544,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H43" sqref="B43:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1566,22 +1606,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
@@ -1589,19 +1629,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -1609,19 +1649,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -1629,19 +1669,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1649,19 +1689,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1669,19 +1709,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -1689,19 +1729,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.3">
@@ -1709,19 +1749,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -1729,19 +1769,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1749,19 +1789,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -1769,16 +1809,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -1787,22 +1827,22 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.3">
@@ -1810,20 +1850,20 @@
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -1831,19 +1871,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -1851,19 +1891,19 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -1871,19 +1911,19 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>114</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.3">
@@ -1891,20 +1931,20 @@
         <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -1912,20 +1952,20 @@
         <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -1933,20 +1973,20 @@
         <v>18</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="15" t="s">
         <v>114</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1954,22 +1994,22 @@
         <v>19</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" s="13">
         <v>20150107</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -1977,22 +2017,22 @@
         <v>20</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="G21" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -2000,22 +2040,22 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="13">
         <v>20150115</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G22" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -2023,22 +2063,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="E23" s="12">
         <v>20150122</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
@@ -2046,22 +2086,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" s="13">
         <v>20150121</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
@@ -2069,19 +2109,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="E25" s="14">
         <v>20150123</v>
       </c>
       <c r="F25" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="H25" s="6"/>
     </row>
@@ -2090,22 +2130,22 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" s="14">
         <v>20150116</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
@@ -2114,19 +2154,19 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E27" s="13">
         <v>20150127</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -2134,22 +2174,22 @@
         <v>27</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="13">
         <v>20150128</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
@@ -2157,19 +2197,19 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E29" s="12">
         <v>20150129</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -2177,22 +2217,22 @@
         <v>29</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E30" s="13">
         <v>20150129</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -2200,22 +2240,22 @@
         <v>30</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="E31" s="13">
         <v>20150129</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G31" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -2223,22 +2263,22 @@
         <v>31</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E32" s="13">
         <v>20150129</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
@@ -2246,22 +2286,22 @@
         <v>32</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E33" s="16">
         <v>20150205</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
@@ -2269,22 +2309,22 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="E34" s="12">
         <v>20150225</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G34" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
@@ -2292,22 +2332,22 @@
         <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="E35" s="14">
         <v>20150225</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
@@ -2315,68 +2355,68 @@
         <v>35</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E36" s="13">
         <v>20150306</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G36" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="6">
+      <c r="B37" s="9">
         <v>36</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="13">
+        <v>20150311</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E37" s="14">
-        <v>20150311</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="9">
+        <v>37</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="D38" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E38" s="13">
+        <v>20150320</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="6">
-        <v>37</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="E38" s="14">
-        <v>20150320</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>228</v>
+      <c r="H38" s="9" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
@@ -2384,22 +2424,22 @@
         <v>38</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E39" s="13">
         <v>20150320</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G39" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="H39" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
@@ -2407,22 +2447,22 @@
         <v>39</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E40" s="13">
         <v>20150320</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
@@ -2430,22 +2470,22 @@
         <v>40</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E41" s="13">
         <v>20150320</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G41" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H41" s="9" t="s">
         <v>223</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
@@ -2453,45 +2493,45 @@
         <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E42" s="12">
         <v>20150319</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H42" s="3" t="s">
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="9">
+        <v>42</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="6">
-        <v>42</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="13">
+        <v>20150318</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="E43" s="14">
-        <v>20150318</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>250</v>
+      <c r="G43" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2499,22 +2539,22 @@
         <v>43</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="E44" s="12">
         <v>20150802</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="21" t="s">
         <v>242</v>
-      </c>
-      <c r="H44" s="21" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
@@ -2522,22 +2562,22 @@
         <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E45" s="12">
         <v>20150812</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
@@ -2590,10 +2630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M36"/>
+  <dimension ref="B1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2616,13 +2656,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
@@ -2642,13 +2682,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -2668,10 +2708,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>8</v>
+        <v>276</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2685,19 +2725,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2711,19 +2751,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2737,19 +2777,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2763,19 +2803,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="F7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2789,16 +2829,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>33</v>
+      <c r="G8" s="3" t="s">
+        <v>277</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2812,19 +2855,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2838,19 +2881,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2864,16 +2907,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2887,19 +2930,19 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2913,19 +2956,19 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2939,16 +2982,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2962,19 +3005,19 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2988,19 +3031,19 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3014,16 +3057,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3037,19 +3080,19 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="F18" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3063,16 +3106,16 @@
         <v>18</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="F19" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="2"/>
@@ -3087,16 +3130,16 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3110,13 +3153,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3130,16 +3173,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3153,16 +3196,16 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3176,16 +3219,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3199,19 +3242,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="E25" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
@@ -3219,16 +3262,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
@@ -3236,19 +3279,19 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
@@ -3256,19 +3299,19 @@
         <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
@@ -3276,16 +3319,16 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
@@ -3293,19 +3336,19 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="E30" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
@@ -3313,19 +3356,19 @@
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>259</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
@@ -3333,75 +3376,124 @@
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="3">
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="3">
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
         <v>35</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="3">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="3">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 add win32 solution file 2 add breadpad so 3 meetplayer gridview title change to 2 lines 4 engine2 remove rtmp optimize code(add macro ENABLE_RTMP_DROP)
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="286">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1153,6 +1153,26 @@
   </si>
   <si>
     <t>system player support snapshot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>大小屏切换时，显示错位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ogl渲染位置有问题，播放先全屏切半屏，或者切换视频源播放会重现</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1584,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H43" sqref="B43:H43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2584,6 +2604,24 @@
       <c r="B46" s="3">
         <v>45</v>
       </c>
+      <c r="C46" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E46" s="12">
+        <v>20151106</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="3">
@@ -2632,7 +2670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1 meetsdk add "ant java"(only build java code and copy meetsdk.jar) 2 meetsdk remove jdom2 dependency 3 foundation support "tiny"(libplayer_neon.so can be 1.8MB) 4 engine2 rtmp protocol add AVFMT_FLAG_NOBUFFER 5 testSDLdlg support SAR aspect ratio
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -11,12 +11,12 @@
     <sheet name="newfeature" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="302">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1173,6 +1173,70 @@
   </si>
   <si>
     <t>ogl渲染位置有问题，播放先全屏切半屏，或者切换视频源播放会重现</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer 部分mp4用ffextrator打开很慢(system 正常)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取 sps pps错误(AVCC解析)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FFPlayer FFExtractor分离</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ffmpeg 裁剪</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer 本地视频拖动慢</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer PPTV视频本地播放SystemMediaExtractor声音不对</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer PPTV视频播放不流畅</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1604,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2627,28 +2691,91 @@
       <c r="B47" s="3">
         <v>46</v>
       </c>
+      <c r="C47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E47" s="12">
+        <v>20151215</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="3">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E48" s="12">
+        <v>20151216</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E49" s="12">
+        <v>20151216</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="3">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E50" s="12">
+        <v>20151216</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="3">
         <v>51</v>
       </c>
@@ -2668,10 +2795,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M38"/>
+  <dimension ref="B1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3532,6 +3659,45 @@
       </c>
       <c r="F38" s="3" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <v>38</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="3">
+        <v>39</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="3">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MeetSDK 1 fix some clip video lag problem(XOPlayer add setVideoAhead()) 2 XOPlayer use FFMediaExtractor for all case(solve some clip video lag, use SystemMediaExtractor cannot solve gracefully)
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="306">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1224,10 +1224,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>tracking</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>XOPlayer 本地视频拖动慢</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1237,6 +1233,26 @@
   </si>
   <si>
     <t>XOPlayer PPTV视频播放不流畅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加video packet的提前量，解决MediaCodec的输入输出限制(influence 网络流实时性变差)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SystemMediaCodec 代码有问题</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIXME SystemMediaCodec 22050 -&gt; 44100 force</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>workaround</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1668,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2724,13 +2740,16 @@
         <v>20151216</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="3">
         <v>48</v>
       </c>
@@ -2744,13 +2763,16 @@
         <v>20151216</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="3">
         <v>49</v>
       </c>
@@ -2764,18 +2786,21 @@
         <v>20151216</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H50" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="3">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
meetsdk 1 fix xiaomi3 1st frame is crash problem when play mp4 file using XOplayer foundation 1 sync win32 build batch
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="309">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1253,6 +1253,18 @@
   </si>
   <si>
     <t>workaround</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer xiaomi3 mp4播放 开始花屏</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>针对MP4等格式 恢复使用bsf h264_mp4toannexb, 原先的替换代码只能适应avpacket中单个nalu unit的case</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1684,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1697,7 +1709,7 @@
     <col min="5" max="5" width="9.75" style="12" customWidth="1"/>
     <col min="6" max="6" width="48.125" style="3" customWidth="1"/>
     <col min="7" max="7" width="8.875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="74.625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="79.75" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2798,6 +2810,24 @@
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
         <v>50</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="12">
+        <v>2015129</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MeetPlayer re-arrange upload log code MeetSDK XOPlayer add release() -> reset() -> stop() logic
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="315">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1212,10 +1212,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>N/A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1265,6 +1261,34 @@
   </si>
   <si>
     <t>针对MP4等格式 恢复使用bsf h264_mp4toannexb, 原先的替换代码只能适应avpacket中单个nalu unit的case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer 网络缓冲中无法中断</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要增加advance() 修改逻辑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhaseI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lite, micro, tiny, gotye(aac_latm need fix)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1330,7 +1354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1393,6 +1417,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1696,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2743,22 +2768,22 @@
         <v>47</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="E48" s="12">
         <v>20151216</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
@@ -2766,22 +2791,22 @@
         <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="E49" s="12">
         <v>20151216</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
@@ -2789,22 +2814,22 @@
         <v>49</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="E50" s="12">
         <v>20151216</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
@@ -2821,18 +2846,36 @@
         <v>2015129</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="H51" s="3" t="s">
+    </row>
+    <row r="52" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="6">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B52" s="3">
-        <v>51</v>
+      <c r="D52" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E52" s="14">
+        <v>20151223</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2852,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3747,7 +3790,10 @@
         <v>294</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>295</v>
+        <v>313</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 MeetPlayer fix getMediaInfo crash 2 MeetSDK XOPlayer fix flv and mkv cannot seek problem 3 MeetSDK XOPlayer solve some ts cann't seek back problem when getTrackFormat()
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="334">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -151,10 +151,6 @@
   </si>
   <si>
     <t>x2 x3 x0.5 x0.25</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统播放器 某些片子也会跳 TBD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -825,14 +821,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>重写XOplayer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PXplayer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ffdemuxer + native MediaCodec(android 5.0+)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -958,10 +946,6 @@
   </si>
   <si>
     <t>第一财经 等频道有时候 seek 后 ，一直缓冲，报a/v 不同步差很多,直接关闭pts_wrap</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PhaseI</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1289,6 +1273,98 @@
   </si>
   <si>
     <t>lite, micro, tiny, gotye(aac_latm need fix)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇家特工480p.mp4 末尾10sec无法播放，自动退出</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer flv/mkv 无法拖动</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统播放器 某些片子也会跳 关键帧位置和seek位置不一致</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>h264_mp4toannexb filter always return error after seek</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer(FFExtractor) support hevc(h265)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PXPlayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhaseII</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重写XOPlayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>support armeabi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer ffextractor find_sps_pps 部分ts获取失败</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1328,7 +1404,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1338,6 +1414,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1354,7 +1436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1418,6 +1500,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1719,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H52"/>
+  <dimension ref="B1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="C55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1742,22 +1835,22 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="24" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1789,16 +1882,16 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -1809,16 +1902,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1832,13 +1925,13 @@
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1852,13 +1945,13 @@
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -1869,16 +1962,16 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.3">
@@ -1889,16 +1982,16 @@
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -1912,13 +2005,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1932,13 +2025,13 @@
         <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -1952,10 +2045,10 @@
         <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -1970,16 +2063,16 @@
         <v>19</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.3">
@@ -1994,13 +2087,13 @@
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -2008,19 +2101,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -2028,19 +2121,19 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -2048,19 +2141,19 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.3">
@@ -2068,20 +2161,20 @@
         <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -2089,20 +2182,20 @@
         <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -2110,20 +2203,20 @@
         <v>18</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G19" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -2131,22 +2224,22 @@
         <v>19</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="13">
         <v>20150107</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -2154,22 +2247,22 @@
         <v>20</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="G21" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -2177,22 +2270,22 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="13">
         <v>20150115</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G22" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
@@ -2200,22 +2293,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="E23" s="12">
         <v>20150122</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
@@ -2223,22 +2316,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24" s="13">
         <v>20150121</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
@@ -2246,19 +2339,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="E25" s="14">
         <v>20150123</v>
       </c>
       <c r="F25" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="H25" s="6"/>
     </row>
@@ -2267,22 +2360,22 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" s="14">
         <v>20150116</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>132</v>
+        <v>319</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
@@ -2291,19 +2384,19 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" s="13">
         <v>20150127</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -2311,22 +2404,22 @@
         <v>27</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="13">
         <v>20150128</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
@@ -2334,19 +2427,19 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="E29" s="12">
         <v>20150129</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -2354,22 +2447,22 @@
         <v>29</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E30" s="13">
         <v>20150129</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -2377,22 +2470,22 @@
         <v>30</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="E31" s="13">
         <v>20150129</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G31" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -2403,19 +2496,19 @@
         <v>9</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E32" s="13">
         <v>20150129</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
@@ -2432,13 +2525,13 @@
         <v>20150205</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
@@ -2446,22 +2539,22 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="E34" s="12">
         <v>20150225</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G34" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
@@ -2469,22 +2562,22 @@
         <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="E35" s="14">
         <v>20150225</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
@@ -2492,22 +2585,22 @@
         <v>35</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E36" s="13">
         <v>20150306</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G36" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
@@ -2515,22 +2608,22 @@
         <v>36</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E37" s="13">
         <v>20150311</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
@@ -2538,22 +2631,22 @@
         <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E38" s="13">
         <v>20150320</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
@@ -2561,22 +2654,22 @@
         <v>38</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E39" s="13">
         <v>20150320</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
@@ -2584,22 +2677,22 @@
         <v>39</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E40" s="13">
         <v>20150320</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
@@ -2607,22 +2700,22 @@
         <v>40</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E41" s="13">
         <v>20150320</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
@@ -2630,22 +2723,22 @@
         <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E42" s="12">
         <v>20150319</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
@@ -2653,22 +2746,22 @@
         <v>42</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E43" s="13">
         <v>20150318</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2676,22 +2769,22 @@
         <v>43</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E44" s="12">
         <v>20150802</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
@@ -2699,22 +2792,22 @@
         <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E45" s="12">
         <v>20150812</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G45" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
@@ -2722,22 +2815,22 @@
         <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E46" s="12">
         <v>20151106</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
@@ -2748,19 +2841,19 @@
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E47" s="12">
         <v>20151215</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
@@ -2768,22 +2861,22 @@
         <v>47</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E48" s="12">
         <v>20151216</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
@@ -2791,22 +2884,22 @@
         <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E49" s="12">
         <v>20151216</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
@@ -2814,22 +2907,22 @@
         <v>49</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E50" s="12">
         <v>20151216</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
@@ -2846,13 +2939,13 @@
         <v>2015129</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -2860,22 +2953,117 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E52" s="14">
         <v>20151223</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="6">
+        <v>52</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="D53" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E53" s="14">
+        <v>20151224</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54" s="3">
+        <v>53</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>312</v>
+      </c>
+      <c r="E54" s="12">
+        <v>20151224</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="6">
+        <v>54</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E55" s="14">
+        <v>20151224</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B58" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B59" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B60" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="3">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2893,10 +3081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M41"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2911,23 +3099,24 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="27" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2"/>
@@ -2937,7 +3126,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -2945,7 +3134,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -2963,7 +3152,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="3">
         <v>2</v>
       </c>
@@ -2971,10 +3160,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2983,7 +3172,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -2991,7 +3180,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -3009,7 +3198,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -3035,7 +3224,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -3061,7 +3250,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>6</v>
       </c>
@@ -3069,16 +3258,16 @@
         <v>28</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -3087,7 +3276,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>7</v>
       </c>
@@ -3095,7 +3284,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>33</v>
@@ -3104,7 +3293,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3113,24 +3302,24 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -3139,24 +3328,24 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3165,21 +3354,21 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3188,24 +3377,24 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3214,24 +3403,24 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3240,21 +3429,21 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3263,24 +3452,24 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -3289,24 +3478,24 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3320,16 +3509,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3343,19 +3532,19 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3369,16 +3558,16 @@
         <v>18</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="F19" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="2"/>
@@ -3393,16 +3582,16 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3416,13 +3605,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3436,16 +3625,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3459,16 +3648,16 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3482,16 +3671,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3505,19 +3694,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="E25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
@@ -3525,16 +3714,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
@@ -3542,19 +3731,19 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="E27" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
@@ -3562,19 +3751,19 @@
         <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
@@ -3582,16 +3771,16 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
@@ -3599,19 +3788,19 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
@@ -3619,19 +3808,19 @@
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
@@ -3639,19 +3828,19 @@
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>261</v>
-      </c>
       <c r="F32" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
@@ -3659,16 +3848,16 @@
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
@@ -3676,16 +3865,16 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
@@ -3693,16 +3882,16 @@
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
@@ -3710,16 +3899,16 @@
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
@@ -3727,19 +3916,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>278</v>
-      </c>
       <c r="F37" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
@@ -3747,16 +3936,16 @@
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
@@ -3764,41 +3953,90 @@
         <v>38</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F39" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="9">
+        <v>39</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="3">
-        <v>39</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>314</v>
+      <c r="F40" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="3">
         <v>40</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="3">
+        <v>41</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="3">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 update gradle 2 fix XOPlayer ffextractor m_buffered_size < 0 bug
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="335">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1244,127 +1244,131 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer 网络缓冲中无法中断</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要增加advance() 修改逻辑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhaseI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lite, micro, tiny, gotye(aac_latm need fix)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>皇家特工480p.mp4 末尾10sec无法播放，自动退出</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tracking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer flv/mkv 无法拖动</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统播放器 某些片子也会跳 关键帧位置和seek位置不一致</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer(FFExtractor) support hevc(h265)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PXPlayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhaseII</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重写XOPlayer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>support armeabi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer ffextractor find_sps_pps 部分ts获取失败</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>针对MP4等格式 恢复使用bsf h264_mp4toannexb, 原先的替换代码只能适应avpacket中单个nalu unit的case</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>N/A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>android</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XOPlayer 网络缓冲中无法中断</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tracking</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要增加advance() 修改逻辑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PhaseI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lite, micro, tiny, gotye(aac_latm need fix)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>android</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>all</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>皇家特工480p.mp4 末尾10sec无法播放，自动退出</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>tracking</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> N/A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XOPlayer flv/mkv 无法拖动</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> tracking</t>
+    <t>nalu start code 存在 3/4 字节2种类型，h264_mp4toannexb 可能导致2种共存</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 h264_mp4toannexb filter update code,2 不试用该filter，自行修改nalu_mp4 -&gt; nalu_annexb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统播放器 某些片子也会跳 关键帧位置和seek位置不一致</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>h264_mp4toannexb filter always return error after seek</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>meetsdk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>android</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XOPlayer(FFExtractor) support hevc(h265)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PXPlayer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PhaseII</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>重写XOPlayer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>support armeabi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>android</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XOPlayer ffextractor find_sps_pps 部分ts获取失败</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1814,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="C55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1891,7 +1895,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -2372,7 +2376,7 @@
         <v>133</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>192</v>
@@ -2945,7 +2949,7 @@
         <v>302</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -2953,22 +2957,22 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="E52" s="14">
         <v>20151223</v>
       </c>
       <c r="F52" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="53" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -2976,19 +2980,19 @@
         <v>52</v>
       </c>
       <c r="C53" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="E53" s="14">
         <v>20151224</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H53" s="6"/>
     </row>
@@ -2997,44 +3001,46 @@
         <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E54" s="12">
         <v>20151224</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>330</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="9">
         <v>54</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="C55" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="E55" s="13">
+        <v>20151224</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="E55" s="14">
-        <v>20151224</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="H55" s="6"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56" s="3">
@@ -3737,10 +3743,10 @@
         <v>196</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>199</v>
@@ -3757,7 +3763,7 @@
         <v>196</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>197</v>
@@ -3979,10 +3985,10 @@
         <v>290</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
@@ -3990,16 +3996,16 @@
         <v>40</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
@@ -4013,10 +4019,10 @@
         <v>19</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 update foundation build batch(support "enc mux librtmp openssl") 2 testEPG/BaiduPanel.java support resumed download 3 use libass(SMP build)
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="342">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1365,6 +1365,34 @@
   </si>
   <si>
     <t>1 h264_mp4toannexb filter update code,2 不试用该filter，自行修改nalu_mp4 -&gt; nalu_annexb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>meetsdk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FFPlayer ogles2 render</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer support no-audio media</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FFPlayer support render filter(ogles2)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1818,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+    <sheetView topLeftCell="D34" workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
@@ -3089,8 +3117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4029,15 +4057,51 @@
       <c r="B43" s="3">
         <v>42</v>
       </c>
+      <c r="C43" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="3">
         <v>43</v>
       </c>
+      <c r="C44" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
         <v>44</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1 MeetSDK fix XOPlayer crash problem(support multi-instance player) 2 MeetPlayer update crash update and breakpad util
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="348">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1397,6 +1397,30 @@
   </si>
   <si>
     <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer 高清视频卡顿</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>read_sample proc 造成 video/audio 读取数据有耦合，无法较好同步。去除多余线程解决</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer 不支持多实例</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改部分 static 变量</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1846,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3074,10 +3098,46 @@
       <c r="B56" s="3">
         <v>55</v>
       </c>
+      <c r="C56" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E56" s="12">
+        <v>20160420</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57" s="3">
         <v>56</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E57" s="12">
+        <v>20160420</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
@@ -3117,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
1 engine2 fix "gotye" build problem 2 meetplayer show actionbar
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="351">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -579,66 +579,62 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>release 1st stable version</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>re-write policy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>need enhance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPBOX-3178</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>某些片子声音播放有很大噪声</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>audioFrame linezize &gt;= nbSample(2048 502)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IOS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>由于编译问题vc1解码模块disabled，导致vc1影片无法播放</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>TBD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>release 1st stable version</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>re-write policy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>need enhance</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPBOX-3178</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>某些片子声音播放有很大噪声</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>audioFrame linezize &gt;= nbSample(2048 502)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>N/A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>IOS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>由于编译问题vc1解码模块disabled，导致vc1影片无法播放</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>android</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -660,10 +656,6 @@
   </si>
   <si>
     <t>扫描本地文件写入db</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1384,10 +1376,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>XOPlayer support no-audio media</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1396,10 +1384,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>N/A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1421,6 +1405,34 @@
   </si>
   <si>
     <t>修改部分 static 变量</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhaseI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHaseI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer support embedded subtitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XOPlayer support ac3 sw decode and play</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1870,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1947,7 +1959,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -2044,7 +2056,7 @@
         <v>54</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>55</v>
@@ -2104,7 +2116,7 @@
         <v>71</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -2169,7 +2181,7 @@
         <v>112</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -2227,10 +2239,10 @@
         <v>88</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -2248,7 +2260,7 @@
         <v>90</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>91</v>
@@ -2315,7 +2327,7 @@
         <v>104</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>127</v>
@@ -2384,7 +2396,7 @@
         <v>125</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>126</v>
@@ -2428,10 +2440,10 @@
         <v>133</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
@@ -2449,10 +2461,10 @@
         <v>135</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -2460,7 +2472,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>80</v>
@@ -2469,13 +2481,13 @@
         <v>20150128</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
@@ -2483,19 +2495,19 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="E29" s="12">
         <v>20150129</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -2503,22 +2515,22 @@
         <v>29</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E30" s="13">
         <v>20150129</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -2526,22 +2538,22 @@
         <v>30</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="E31" s="13">
         <v>20150129</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -2552,19 +2564,19 @@
         <v>9</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E32" s="13">
         <v>20150129</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G32" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
@@ -2581,13 +2593,13 @@
         <v>20150205</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
@@ -2595,22 +2607,22 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E34" s="12">
         <v>20150225</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
@@ -2618,22 +2630,22 @@
         <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E35" s="14">
         <v>20150225</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>123</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
@@ -2641,22 +2653,22 @@
         <v>35</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E36" s="13">
         <v>20150306</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
@@ -2664,22 +2676,22 @@
         <v>36</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E37" s="13">
         <v>20150311</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
@@ -2687,22 +2699,22 @@
         <v>37</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E38" s="13">
         <v>20150320</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
@@ -2710,22 +2722,22 @@
         <v>38</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E39" s="13">
         <v>20150320</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
@@ -2733,22 +2745,22 @@
         <v>39</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E40" s="13">
         <v>20150320</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G40" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H40" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
@@ -2756,22 +2768,22 @@
         <v>40</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E41" s="13">
         <v>20150320</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
@@ -2779,22 +2791,22 @@
         <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E42" s="12">
         <v>20150319</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
@@ -2802,22 +2814,22 @@
         <v>42</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E43" s="13">
         <v>20150318</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2825,22 +2837,22 @@
         <v>43</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E44" s="12">
         <v>20150802</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H44" s="21" t="s">
         <v>236</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H44" s="21" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
@@ -2848,22 +2860,22 @@
         <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E45" s="12">
         <v>20150812</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
@@ -2871,22 +2883,22 @@
         <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E46" s="12">
         <v>20151106</v>
       </c>
       <c r="F46" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
@@ -2897,19 +2909,19 @@
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E47" s="12">
         <v>20151215</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G47" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
@@ -2917,22 +2929,22 @@
         <v>47</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E48" s="12">
         <v>20151216</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G48" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
@@ -2940,22 +2952,22 @@
         <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E49" s="12">
         <v>20151216</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
@@ -2963,22 +2975,22 @@
         <v>49</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E50" s="12">
         <v>20151216</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
@@ -2995,13 +3007,13 @@
         <v>2015129</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="52" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -3009,22 +3021,22 @@
         <v>51</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E52" s="14">
         <v>20151223</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53" spans="2:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -3032,19 +3044,19 @@
         <v>52</v>
       </c>
       <c r="C53" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>309</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="E53" s="14">
         <v>20151224</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H53" s="6"/>
     </row>
@@ -3053,22 +3065,22 @@
         <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E54" s="12">
         <v>20151224</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="2:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -3076,22 +3088,22 @@
         <v>54</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E55" s="13">
         <v>20151224</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G55" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="H55" s="9" t="s">
         <v>330</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
@@ -3099,22 +3111,22 @@
         <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E56" s="12">
         <v>20160420</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
@@ -3122,22 +3134,22 @@
         <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E57" s="12">
         <v>20160420</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
@@ -3175,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3257,7 +3269,7 @@
         <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -3358,10 +3370,10 @@
         <v>29</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -3387,7 +3399,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3407,10 +3419,10 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>34</v>
@@ -3436,10 +3448,10 @@
         <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>227</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>229</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3462,7 +3474,7 @@
         <v>38</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3583,13 +3595,13 @@
         <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3609,10 +3621,10 @@
         <v>59</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3635,10 +3647,10 @@
         <v>70</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3685,7 +3697,7 @@
         <v>74</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3705,7 +3717,7 @@
         <v>75</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3728,7 +3740,7 @@
         <v>137</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>138</v>
+        <v>345</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3742,16 +3754,16 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>159</v>
+        <v>345</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3765,16 +3777,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3788,19 +3800,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
@@ -3808,16 +3820,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
@@ -3825,19 +3837,19 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
@@ -3845,19 +3857,19 @@
         <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
@@ -3865,16 +3877,16 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
@@ -3882,19 +3894,19 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
@@ -3902,19 +3914,19 @@
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
@@ -3922,19 +3934,19 @@
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
@@ -3942,16 +3954,16 @@
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
@@ -3959,16 +3971,16 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
@@ -3976,16 +3988,16 @@
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
@@ -3993,16 +4005,16 @@
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
@@ -4010,19 +4022,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>271</v>
-      </c>
       <c r="G37" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
@@ -4030,16 +4042,16 @@
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
@@ -4053,10 +4065,10 @@
         <v>19</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="2:7" s="23" customFormat="1" x14ac:dyDescent="0.3">
@@ -4064,19 +4076,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>290</v>
-      </c>
       <c r="F40" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
@@ -4084,16 +4096,16 @@
         <v>40</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
@@ -4107,10 +4119,10 @@
         <v>19</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
@@ -4118,16 +4130,16 @@
         <v>42</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="F43" s="3" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
@@ -4135,16 +4147,16 @@
         <v>43</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>339</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
@@ -4152,21 +4164,60 @@
         <v>44</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="3">
         <v>45</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="3">
+        <v>46</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="3">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 meetplayer add DMCActivity 2 foundation add build_ffplay.txt
</commit_message>
<xml_diff>
--- a/engine2/Doc/buglist&newfeature.xlsx
+++ b/engine2/Doc/buglist&newfeature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="bug" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="F59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+08-04 16:22:14.278 7107-7217/? I/FFExtractor: audio codec: codec_id 86018, channels 2, channel_layout 3, sample_rate 44100, sample_fmt -1
+08-04 16:25:36.518 7645-7674/? I/FFExtractor: audio codec: codec_id 86018, channels 1, channel_layout 4, sample_rate 44100, sample_fmt 8</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="359">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1433,6 +1468,38 @@
   </si>
   <si>
     <t>XOPlayer support ac3 sw decode and play</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌兰托娅 - 套马杆.ape 时间戳不连续。有1s多间隔</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">audio_decode ret =0,0,0,0,xxxx,0,0,0,yyyy 即使output&gt;1，ret也不&gt;0 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>foundation "gotye" build xoplayer aac channel incorrect</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>enable-parser=aac,aac_latm enable-decoder=aac_latm</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1443,7 +1510,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1469,6 +1536,19 @@
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1879,11 +1959,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3156,10 +3236,46 @@
       <c r="B58" s="3">
         <v>57</v>
       </c>
+      <c r="C58" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E58" s="12">
+        <v>20160725</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="3">
         <v>58</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E59" s="12">
+        <v>20160804</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
@@ -3182,6 +3298,7 @@
   <ignoredErrors>
     <ignoredError sqref="E12 E21" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3189,7 +3306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>